<commit_message>
more changes to figures
</commit_message>
<xml_diff>
--- a/figures/features.xlsx
+++ b/figures/features.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Features</t>
+    <t xml:space="preserve">Feature Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Features</t>
   </si>
   <si>
     <t xml:space="preserve">Non-descriptive</t>
@@ -205,13 +205,13 @@
   </sheetPr>
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="63.21"/>
   </cols>
   <sheetData>

</xml_diff>